<commit_message>
Update call number ranges for MAIN L4 books
</commit_message>
<xml_diff>
--- a/utils/datastore_from_xlsx_sample_input.xlsx
+++ b/utils/datastore_from_xlsx_sample_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7170" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16890" windowHeight="6810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Libraries" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="510">
   <si>
     <t>_id</t>
   </si>
@@ -1292,6 +1292,270 @@
   </si>
   <si>
     <t>LC149.5 .E16 2015</t>
+  </si>
+  <si>
+    <t>AC25 .B3132 1972</t>
+  </si>
+  <si>
+    <t>B382 .A5 T39 1996</t>
+  </si>
+  <si>
+    <t>B384 .H4513 1997</t>
+  </si>
+  <si>
+    <t>B851 .B49 2004</t>
+  </si>
+  <si>
+    <t>B905 .T73 2001</t>
+  </si>
+  <si>
+    <t>B3376 .W563 T7313 2001</t>
+  </si>
+  <si>
+    <t>B3376 .W564 C56 1999</t>
+  </si>
+  <si>
+    <t>BD216 .M58 2009</t>
+  </si>
+  <si>
+    <t>BD220 .B86 2010</t>
+  </si>
+  <si>
+    <t>BF81 .V37 2011</t>
+  </si>
+  <si>
+    <t>BF95 .B43 2007</t>
+  </si>
+  <si>
+    <t>BF341 .P47 2002</t>
+  </si>
+  <si>
+    <t>BF353 .B6613 1995</t>
+  </si>
+  <si>
+    <t>BF531 .P36 2012</t>
+  </si>
+  <si>
+    <t>BF698 .A3614 2000</t>
+  </si>
+  <si>
+    <t>BF698 .B73 1998</t>
+  </si>
+  <si>
+    <t>BJ1025 .W43 1997</t>
+  </si>
+  <si>
+    <t>BJ1031 .A48 2002</t>
+  </si>
+  <si>
+    <t>BL1201 .C42 2011</t>
+  </si>
+  <si>
+    <t>BL1202 .B72 2005</t>
+  </si>
+  <si>
+    <t>BQ4133 .P363 2004</t>
+  </si>
+  <si>
+    <t>BQ4150 .G69 2003</t>
+  </si>
+  <si>
+    <t>CB481 .S58 1998</t>
+  </si>
+  <si>
+    <t>CC72.4 .M55 1987</t>
+  </si>
+  <si>
+    <t>D839.7 .A56 M45 2007</t>
+  </si>
+  <si>
+    <t>D840 .S68 2010</t>
+  </si>
+  <si>
+    <t>DS79.76 .H652 2008</t>
+  </si>
+  <si>
+    <t>DS79.76 .W37 2003</t>
+  </si>
+  <si>
+    <t>DS530.4 .S65 1999</t>
+  </si>
+  <si>
+    <t>DS530.53 .A85 A86 2008</t>
+  </si>
+  <si>
+    <t>DS644.5 .G68 2003</t>
+  </si>
+  <si>
+    <t>DS644.5 .I525 2001</t>
+  </si>
+  <si>
+    <t>DS830 .J37 2002</t>
+  </si>
+  <si>
+    <t>DS830 .K345 1991</t>
+  </si>
+  <si>
+    <t>E895 .A44 2002</t>
+  </si>
+  <si>
+    <t>E895 .B79 2004</t>
+  </si>
+  <si>
+    <t>GN346 .L44 1995</t>
+  </si>
+  <si>
+    <t>GN346 .R43 2013</t>
+  </si>
+  <si>
+    <t>GV1588.6 .T46 1995</t>
+  </si>
+  <si>
+    <t>GV1589 .I53 2008</t>
+  </si>
+  <si>
+    <t>HB34 .P423 1996</t>
+  </si>
+  <si>
+    <t>HB61 .B33 1998</t>
+  </si>
+  <si>
+    <t>HB137 .R36 1993</t>
+  </si>
+  <si>
+    <t>HB139 .A324 1995</t>
+  </si>
+  <si>
+    <t>HB171 .M545 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HB172.5 .S5269 2001 </t>
+  </si>
+  <si>
+    <t>HB172.5 .S648 1999</t>
+  </si>
+  <si>
+    <t>HB615 .L265 2007</t>
+  </si>
+  <si>
+    <t>HB615 .L457 2009</t>
+  </si>
+  <si>
+    <t>HB3808 .S63 2001</t>
+  </si>
+  <si>
+    <t>HB3808 .S87 2000</t>
+  </si>
+  <si>
+    <t>HC79 .I55 S685 2017</t>
+  </si>
+  <si>
+    <t>HC79 .I55 T36 2002</t>
+  </si>
+  <si>
+    <t>HC310 .D5 G56 2001</t>
+  </si>
+  <si>
+    <t>HC336.27 .L68 2004</t>
+  </si>
+  <si>
+    <t>HC430 .H53 G82 2006</t>
+  </si>
+  <si>
+    <t>HC430 .H53 N55 2009</t>
+  </si>
+  <si>
+    <t>HC460.5 .T56 1998</t>
+  </si>
+  <si>
+    <t>HC460.5 .T695 2005</t>
+  </si>
+  <si>
+    <t>HD30.2 .W464 2007</t>
+  </si>
+  <si>
+    <t>HD30.2 .W56 2003</t>
+  </si>
+  <si>
+    <t>HD30.28 .H36656 2002</t>
+  </si>
+  <si>
+    <t>HD30.28 .H3786 2002</t>
+  </si>
+  <si>
+    <t>HD31 .F564 1978</t>
+  </si>
+  <si>
+    <t>HD31 .F74 2012</t>
+  </si>
+  <si>
+    <t>HD49 .C35 2002</t>
+  </si>
+  <si>
+    <t>HD49 .C37 2000</t>
+  </si>
+  <si>
+    <t>HD57.7 .S835 2008</t>
+  </si>
+  <si>
+    <t>HD57.7 .T49 2004</t>
+  </si>
+  <si>
+    <t>HD58.8 .N63 1993</t>
+  </si>
+  <si>
+    <t>HD61 .G57 2000</t>
+  </si>
+  <si>
+    <t>HD61 .G667 2004</t>
+  </si>
+  <si>
+    <t>HD62.7 .Z55 2011</t>
+  </si>
+  <si>
+    <t>HD66 .A383 1997 v.4</t>
+  </si>
+  <si>
+    <t>HD75 .I57 2006</t>
+  </si>
+  <si>
+    <t>HD75 .K46 2011</t>
+  </si>
+  <si>
+    <t>HD2385 .I5 W48 2004</t>
+  </si>
+  <si>
+    <t>HD2721 .M286 2008</t>
+  </si>
+  <si>
+    <t>HD3616 .E184 A24 1990</t>
+  </si>
+  <si>
+    <t>HD3616 .E8 K37 1985</t>
+  </si>
+  <si>
+    <t>HD7096 .J3 E26 2004</t>
+  </si>
+  <si>
+    <t>HD7103.65 .S55 F55 2017</t>
+  </si>
+  <si>
+    <t>HD9696.8 .U63 N745 2004</t>
+  </si>
+  <si>
+    <t>HD9696.8 .U64 B73 2011</t>
+  </si>
+  <si>
+    <t>HE9897.8 .P52 1989</t>
+  </si>
+  <si>
+    <t>HD58.8 .O37 1998</t>
+  </si>
+  <si>
+    <t>HB171 .M558 2013</t>
+  </si>
+  <si>
+    <t>BF531 .O94 2009</t>
   </si>
 </sst>
 </file>
@@ -1970,9 +2234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2048,8 +2310,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="1" t="b">
-        <f>F5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2091,7 +2352,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2573,7 +2834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4201,13 +4462,13 @@
       <c r="D48" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="3" t="str">
         <f t="shared" ref="E48:F48" si="44">E138</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="3">
+        <v>AC25 .B3132 1972</v>
+      </c>
+      <c r="F48" s="3" t="str">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>B382 .A5 T39 1996</v>
       </c>
       <c r="G48" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4218,7 +4479,7 @@
       </c>
       <c r="I48" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4235,13 +4496,13 @@
       <c r="D49" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="3" t="str">
         <f t="shared" ref="E49:F49" si="45">E139</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="3">
+        <v>B384 .H4513 1997</v>
+      </c>
+      <c r="F49" s="3" t="str">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>B851 .B49 2004</v>
       </c>
       <c r="G49" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4252,7 +4513,7 @@
       </c>
       <c r="I49" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4269,13 +4530,13 @@
       <c r="D50" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="3" t="str">
         <f t="shared" ref="E50:F50" si="46">E140</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="3">
+        <v>B905 .T73 2001</v>
+      </c>
+      <c r="F50" s="3" t="str">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>B3376 .W563 T7313 2001</v>
       </c>
       <c r="G50" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4286,7 +4547,7 @@
       </c>
       <c r="I50" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4303,13 +4564,13 @@
       <c r="D51" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="3" t="str">
         <f t="shared" ref="E51:F51" si="47">E141</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="3">
+        <v>B3376 .W564 C56 1999</v>
+      </c>
+      <c r="F51" s="3" t="str">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>BD216 .M58 2009</v>
       </c>
       <c r="G51" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4320,7 +4581,7 @@
       </c>
       <c r="I51" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4337,13 +4598,13 @@
       <c r="D52" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="3" t="str">
         <f t="shared" ref="E52:F52" si="48">E142</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="3">
+        <v>BD220 .B86 2010</v>
+      </c>
+      <c r="F52" s="3" t="str">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>BF81 .V37 2011</v>
       </c>
       <c r="G52" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4354,7 +4615,7 @@
       </c>
       <c r="I52" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4371,13 +4632,13 @@
       <c r="D53" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="3" t="str">
         <f t="shared" ref="E53:F53" si="49">E143</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="3">
+        <v>BF95 .B43 2007</v>
+      </c>
+      <c r="F53" s="3" t="str">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>BF341 .P47 2002</v>
       </c>
       <c r="G53" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4387,8 +4648,8 @@
         <v>187</v>
       </c>
       <c r="I53" s="4" t="b">
-        <f>I143</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4405,13 +4666,13 @@
       <c r="D54" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="3" t="str">
         <f t="shared" ref="E54:F54" si="50">E144</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="3">
+        <v>BF353 .B6613 1995</v>
+      </c>
+      <c r="F54" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>BF531 .O94 2009</v>
       </c>
       <c r="G54" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4422,7 +4683,7 @@
       </c>
       <c r="I54" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4439,13 +4700,13 @@
       <c r="D55" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="3" t="str">
         <f t="shared" ref="E55:F55" si="51">E145</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="3">
+        <v>BF531 .P36 2012</v>
+      </c>
+      <c r="F55" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>BF698 .A3614 2000</v>
       </c>
       <c r="G55" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4456,7 +4717,7 @@
       </c>
       <c r="I55" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4473,13 +4734,13 @@
       <c r="D56" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="3" t="str">
         <f t="shared" ref="E56:F56" si="52">E146</f>
-        <v>0</v>
-      </c>
-      <c r="F56" s="3">
+        <v>BF698 .B73 1998</v>
+      </c>
+      <c r="F56" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>BJ1025 .W43 1997</v>
       </c>
       <c r="G56" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4490,7 +4751,7 @@
       </c>
       <c r="I56" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4507,13 +4768,13 @@
       <c r="D57" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="3" t="str">
         <f t="shared" ref="E57:F57" si="53">E147</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="3">
+        <v>BJ1031 .A48 2002</v>
+      </c>
+      <c r="F57" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>BL1201 .C42 2011</v>
       </c>
       <c r="G57" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4524,7 +4785,7 @@
       </c>
       <c r="I57" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -4541,13 +4802,13 @@
       <c r="D58" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="3" t="str">
         <f t="shared" ref="E58:F58" si="54">E148</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="3">
+        <v>BL1202 .B72 2005</v>
+      </c>
+      <c r="F58" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>BQ4133 .P363 2004</v>
       </c>
       <c r="G58" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4558,7 +4819,7 @@
       </c>
       <c r="I58" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -4575,13 +4836,13 @@
       <c r="D59" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="3" t="str">
         <f t="shared" ref="E59:F59" si="55">E149</f>
-        <v>0</v>
-      </c>
-      <c r="F59" s="3">
+        <v>BQ4150 .G69 2003</v>
+      </c>
+      <c r="F59" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>CB481 .S58 1998</v>
       </c>
       <c r="G59" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4592,7 +4853,7 @@
       </c>
       <c r="I59" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -4609,13 +4870,13 @@
       <c r="D60" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="3" t="str">
         <f t="shared" ref="E60:F60" si="56">E150</f>
-        <v>0</v>
-      </c>
-      <c r="F60" s="3">
+        <v>CC72.4 .M55 1987</v>
+      </c>
+      <c r="F60" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>D839.7 .A56 M45 2007</v>
       </c>
       <c r="G60" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4626,7 +4887,7 @@
       </c>
       <c r="I60" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -4643,13 +4904,13 @@
       <c r="D61" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="3" t="str">
         <f t="shared" ref="E61:F61" si="57">E151</f>
-        <v>0</v>
-      </c>
-      <c r="F61" s="3">
+        <v>D840 .S68 2010</v>
+      </c>
+      <c r="F61" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>DS79.76 .H652 2008</v>
       </c>
       <c r="G61" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4660,7 +4921,7 @@
       </c>
       <c r="I61" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -4677,13 +4938,13 @@
       <c r="D62" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="3" t="str">
         <f t="shared" ref="E62:F62" si="58">E152</f>
-        <v>0</v>
-      </c>
-      <c r="F62" s="3">
+        <v>DS79.76 .W37 2003</v>
+      </c>
+      <c r="F62" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>DS530.4 .S65 1999</v>
       </c>
       <c r="G62" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4694,7 +4955,7 @@
       </c>
       <c r="I62" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -4711,13 +4972,13 @@
       <c r="D63" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="3" t="str">
         <f t="shared" ref="E63:F63" si="59">E153</f>
-        <v>0</v>
-      </c>
-      <c r="F63" s="3">
+        <v>DS530.53 .A85 A86 2008</v>
+      </c>
+      <c r="F63" s="3" t="str">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>DS644.5 .G68 2003</v>
       </c>
       <c r="G63" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4728,7 +4989,7 @@
       </c>
       <c r="I63" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -4745,13 +5006,13 @@
       <c r="D64" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="3" t="str">
         <f t="shared" ref="E64:F64" si="60">E154</f>
-        <v>0</v>
-      </c>
-      <c r="F64" s="3">
+        <v>DS644.5 .I525 2001</v>
+      </c>
+      <c r="F64" s="3" t="str">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>DS830 .J37 2002</v>
       </c>
       <c r="G64" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4762,7 +5023,7 @@
       </c>
       <c r="I64" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -4779,13 +5040,13 @@
       <c r="D65" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="3" t="str">
         <f t="shared" ref="E65:F65" si="61">E155</f>
-        <v>0</v>
-      </c>
-      <c r="F65" s="3">
+        <v>DS830 .K345 1991</v>
+      </c>
+      <c r="F65" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>E895 .A44 2002</v>
       </c>
       <c r="G65" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4796,7 +5057,7 @@
       </c>
       <c r="I65" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4813,13 +5074,13 @@
       <c r="D66" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="3" t="str">
         <f t="shared" ref="E66:F66" si="62">E156</f>
-        <v>0</v>
-      </c>
-      <c r="F66" s="3">
+        <v>E895 .B79 2004</v>
+      </c>
+      <c r="F66" s="3" t="str">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>GN346 .L44 1995</v>
       </c>
       <c r="G66" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4830,7 +5091,7 @@
       </c>
       <c r="I66" s="4" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4847,13 +5108,13 @@
       <c r="D67" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="3" t="str">
         <f t="shared" ref="E67:F67" si="63">E157</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="3">
+        <v>GN346 .R43 2013</v>
+      </c>
+      <c r="F67" s="3" t="str">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>GV1588.6 .T46 1995</v>
       </c>
       <c r="G67" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4863,8 +5124,8 @@
         <v>187</v>
       </c>
       <c r="I67" s="4" t="b">
-        <f t="shared" ref="I67:I78" si="64">I157</f>
-        <v>0</v>
+        <f t="shared" ref="I67" si="64">I157</f>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -4881,13 +5142,13 @@
       <c r="D68" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="3" t="str">
         <f t="shared" ref="E68:F68" si="65">E158</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="3">
+        <v>GV1589 .I53 2008</v>
+      </c>
+      <c r="F68" s="3" t="str">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>HB34 .P423 1996</v>
       </c>
       <c r="G68" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4897,8 +5158,8 @@
         <v>187</v>
       </c>
       <c r="I68" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" ref="I67:I78" si="66">I158</f>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -4915,13 +5176,13 @@
       <c r="D69" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E69" s="3">
-        <f t="shared" ref="E69:F69" si="66">E159</f>
-        <v>0</v>
-      </c>
-      <c r="F69" s="3">
-        <f t="shared" si="66"/>
-        <v>0</v>
+      <c r="E69" s="3" t="str">
+        <f t="shared" ref="E69:F69" si="67">E159</f>
+        <v>HB61 .B33 1998</v>
+      </c>
+      <c r="F69" s="3" t="str">
+        <f t="shared" si="67"/>
+        <v>HB137 .R36 1993</v>
       </c>
       <c r="G69" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4931,8 +5192,8 @@
         <v>187</v>
       </c>
       <c r="I69" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -4949,13 +5210,13 @@
       <c r="D70" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E70" s="3">
-        <f t="shared" ref="E70:F70" si="67">E160</f>
-        <v>0</v>
-      </c>
-      <c r="F70" s="3">
-        <f t="shared" si="67"/>
-        <v>0</v>
+      <c r="E70" s="3" t="str">
+        <f t="shared" ref="E70:F70" si="68">E160</f>
+        <v>HB139 .A324 1995</v>
+      </c>
+      <c r="F70" s="3" t="str">
+        <f t="shared" si="68"/>
+        <v>HB171 .M545 2009</v>
       </c>
       <c r="G70" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4965,8 +5226,8 @@
         <v>187</v>
       </c>
       <c r="I70" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -4983,13 +5244,13 @@
       <c r="D71" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E71" s="3">
-        <f t="shared" ref="E71:F71" si="68">E161</f>
-        <v>0</v>
-      </c>
-      <c r="F71" s="3">
-        <f t="shared" si="68"/>
-        <v>0</v>
+      <c r="E71" s="3" t="str">
+        <f t="shared" ref="E71:F71" si="69">E161</f>
+        <v>HB171 .M558 2013</v>
+      </c>
+      <c r="F71" s="3" t="str">
+        <f t="shared" si="69"/>
+        <v xml:space="preserve">HB172.5 .S5269 2001 </v>
       </c>
       <c r="G71" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -4999,8 +5260,8 @@
         <v>187</v>
       </c>
       <c r="I71" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -5017,13 +5278,13 @@
       <c r="D72" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E72" s="3">
-        <f t="shared" ref="E72:F72" si="69">E162</f>
-        <v>0</v>
-      </c>
-      <c r="F72" s="3">
-        <f t="shared" si="69"/>
-        <v>0</v>
+      <c r="E72" s="3" t="str">
+        <f t="shared" ref="E72:F72" si="70">E162</f>
+        <v>HB172.5 .S648 1999</v>
+      </c>
+      <c r="F72" s="3" t="str">
+        <f t="shared" si="70"/>
+        <v>HB615 .L265 2007</v>
       </c>
       <c r="G72" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5033,8 +5294,8 @@
         <v>187</v>
       </c>
       <c r="I72" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -5051,13 +5312,13 @@
       <c r="D73" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E73" s="3">
-        <f t="shared" ref="E73:F73" si="70">E163</f>
-        <v>0</v>
-      </c>
-      <c r="F73" s="3">
-        <f t="shared" si="70"/>
-        <v>0</v>
+      <c r="E73" s="3" t="str">
+        <f t="shared" ref="E73:F73" si="71">E163</f>
+        <v>HB615 .L457 2009</v>
+      </c>
+      <c r="F73" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>HB3808 .S63 2001</v>
       </c>
       <c r="G73" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5067,8 +5328,8 @@
         <v>187</v>
       </c>
       <c r="I73" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -5085,13 +5346,13 @@
       <c r="D74" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E74" s="3">
-        <f t="shared" ref="E74:F74" si="71">E164</f>
-        <v>0</v>
-      </c>
-      <c r="F74" s="3">
-        <f t="shared" si="71"/>
-        <v>0</v>
+      <c r="E74" s="3" t="str">
+        <f t="shared" ref="E74:F74" si="72">E164</f>
+        <v>HB3808 .S87 2000</v>
+      </c>
+      <c r="F74" s="3" t="str">
+        <f t="shared" si="72"/>
+        <v>HC79 .I55 S685 2017</v>
       </c>
       <c r="G74" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5101,8 +5362,8 @@
         <v>187</v>
       </c>
       <c r="I74" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -5119,13 +5380,13 @@
       <c r="D75" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E75" s="3">
-        <f t="shared" ref="E75:F75" si="72">E165</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="3">
-        <f t="shared" si="72"/>
-        <v>0</v>
+      <c r="E75" s="3" t="str">
+        <f t="shared" ref="E75:F75" si="73">E165</f>
+        <v>HC79 .I55 T36 2002</v>
+      </c>
+      <c r="F75" s="3" t="str">
+        <f t="shared" si="73"/>
+        <v>HC310 .D5 G56 2001</v>
       </c>
       <c r="G75" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5135,8 +5396,8 @@
         <v>187</v>
       </c>
       <c r="I75" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -5153,13 +5414,13 @@
       <c r="D76" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E76" s="3">
-        <f t="shared" ref="E76:F76" si="73">E166</f>
-        <v>0</v>
-      </c>
-      <c r="F76" s="3">
-        <f t="shared" si="73"/>
-        <v>0</v>
+      <c r="E76" s="3" t="str">
+        <f t="shared" ref="E76:F76" si="74">E166</f>
+        <v>HC336.27 .L68 2004</v>
+      </c>
+      <c r="F76" s="3" t="str">
+        <f t="shared" si="74"/>
+        <v>HC430 .H53 G82 2006</v>
       </c>
       <c r="G76" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5169,8 +5430,8 @@
         <v>187</v>
       </c>
       <c r="I76" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -5187,13 +5448,13 @@
       <c r="D77" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E77" s="3">
-        <f t="shared" ref="E77:F77" si="74">E167</f>
-        <v>0</v>
-      </c>
-      <c r="F77" s="3">
-        <f t="shared" si="74"/>
-        <v>0</v>
+      <c r="E77" s="3" t="str">
+        <f t="shared" ref="E77:F77" si="75">E167</f>
+        <v>HC430 .H53 N55 2009</v>
+      </c>
+      <c r="F77" s="3" t="str">
+        <f t="shared" si="75"/>
+        <v>HC460.5 .T56 1998</v>
       </c>
       <c r="G77" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5203,8 +5464,8 @@
         <v>187</v>
       </c>
       <c r="I77" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5221,13 +5482,13 @@
       <c r="D78" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E78" s="3">
-        <f t="shared" ref="E78:F78" si="75">E168</f>
-        <v>0</v>
-      </c>
-      <c r="F78" s="3">
-        <f t="shared" si="75"/>
-        <v>0</v>
+      <c r="E78" s="3" t="str">
+        <f t="shared" ref="E78:F78" si="76">E168</f>
+        <v>HC460.5 .T695 2005</v>
+      </c>
+      <c r="F78" s="3" t="str">
+        <f t="shared" si="76"/>
+        <v>HD30.2 .W464 2007</v>
       </c>
       <c r="G78" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5237,8 +5498,8 @@
         <v>187</v>
       </c>
       <c r="I78" s="4" t="b">
-        <f t="shared" si="64"/>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -5255,13 +5516,13 @@
       <c r="D79" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E79" s="3">
-        <f t="shared" ref="E79:F79" si="76">E169</f>
-        <v>0</v>
-      </c>
-      <c r="F79" s="3">
-        <f t="shared" si="76"/>
-        <v>0</v>
+      <c r="E79" s="3" t="str">
+        <f t="shared" ref="E79:F79" si="77">E169</f>
+        <v>HD30.2 .W56 2003</v>
+      </c>
+      <c r="F79" s="3" t="str">
+        <f t="shared" si="77"/>
+        <v>HD30.28 .H36656 2002</v>
       </c>
       <c r="G79" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5272,7 +5533,7 @@
       </c>
       <c r="I79" s="4" t="b">
         <f>I169</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -5289,13 +5550,13 @@
       <c r="D80" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E80" s="3">
-        <f t="shared" ref="E80:F80" si="77">E170</f>
-        <v>0</v>
-      </c>
-      <c r="F80" s="3">
-        <f t="shared" si="77"/>
-        <v>0</v>
+      <c r="E80" s="3" t="str">
+        <f t="shared" ref="E80:F80" si="78">E170</f>
+        <v>HD30.28 .H3786 2002</v>
+      </c>
+      <c r="F80" s="3" t="str">
+        <f t="shared" si="78"/>
+        <v>HD31 .F564 1978</v>
       </c>
       <c r="G80" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5305,8 +5566,8 @@
         <v>187</v>
       </c>
       <c r="I80" s="4" t="b">
-        <f t="shared" ref="I80:I91" si="78">I170</f>
-        <v>0</v>
+        <f t="shared" ref="I80:I91" si="79">I170</f>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -5323,13 +5584,13 @@
       <c r="D81" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E81" s="3">
-        <f t="shared" ref="E81:F81" si="79">E171</f>
-        <v>0</v>
-      </c>
-      <c r="F81" s="3">
-        <f t="shared" si="79"/>
-        <v>0</v>
+      <c r="E81" s="3" t="str">
+        <f t="shared" ref="E81:F81" si="80">E171</f>
+        <v>HD31 .F74 2012</v>
+      </c>
+      <c r="F81" s="3" t="str">
+        <f t="shared" si="80"/>
+        <v>HD49 .C35 2002</v>
       </c>
       <c r="G81" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5339,8 +5600,8 @@
         <v>187</v>
       </c>
       <c r="I81" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -5357,13 +5618,13 @@
       <c r="D82" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E82" s="3">
-        <f t="shared" ref="E82:F82" si="80">E172</f>
-        <v>0</v>
-      </c>
-      <c r="F82" s="3">
-        <f t="shared" si="80"/>
-        <v>0</v>
+      <c r="E82" s="3" t="str">
+        <f t="shared" ref="E82:F82" si="81">E172</f>
+        <v>HD49 .C37 2000</v>
+      </c>
+      <c r="F82" s="3" t="str">
+        <f t="shared" si="81"/>
+        <v>HD57.7 .S835 2008</v>
       </c>
       <c r="G82" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5373,8 +5634,8 @@
         <v>187</v>
       </c>
       <c r="I82" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -5391,13 +5652,13 @@
       <c r="D83" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E83" s="3">
-        <f t="shared" ref="E83:F83" si="81">E173</f>
-        <v>0</v>
-      </c>
-      <c r="F83" s="3">
-        <f t="shared" si="81"/>
-        <v>0</v>
+      <c r="E83" s="3" t="str">
+        <f t="shared" ref="E83:F83" si="82">E173</f>
+        <v>HD57.7 .T49 2004</v>
+      </c>
+      <c r="F83" s="3" t="str">
+        <f t="shared" si="82"/>
+        <v>HD58.8 .N63 1993</v>
       </c>
       <c r="G83" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5407,8 +5668,8 @@
         <v>187</v>
       </c>
       <c r="I83" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -5425,13 +5686,13 @@
       <c r="D84" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E84" s="3">
-        <f t="shared" ref="E84:F84" si="82">E174</f>
-        <v>0</v>
-      </c>
-      <c r="F84" s="3">
-        <f t="shared" si="82"/>
-        <v>0</v>
+      <c r="E84" s="3" t="str">
+        <f t="shared" ref="E84:F84" si="83">E174</f>
+        <v>HD58.8 .O37 1998</v>
+      </c>
+      <c r="F84" s="3" t="str">
+        <f t="shared" si="83"/>
+        <v>HD61 .G57 2000</v>
       </c>
       <c r="G84" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5441,8 +5702,8 @@
         <v>187</v>
       </c>
       <c r="I84" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -5459,13 +5720,13 @@
       <c r="D85" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E85" s="3">
-        <f t="shared" ref="E85:F85" si="83">E175</f>
-        <v>0</v>
-      </c>
-      <c r="F85" s="3">
-        <f t="shared" si="83"/>
-        <v>0</v>
+      <c r="E85" s="3" t="str">
+        <f t="shared" ref="E85:F85" si="84">E175</f>
+        <v>HD61 .G667 2004</v>
+      </c>
+      <c r="F85" s="3" t="str">
+        <f t="shared" si="84"/>
+        <v>HD62.7 .Z55 2011</v>
       </c>
       <c r="G85" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5475,8 +5736,8 @@
         <v>187</v>
       </c>
       <c r="I85" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -5493,13 +5754,13 @@
       <c r="D86" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E86" s="3">
-        <f t="shared" ref="E86:F86" si="84">E176</f>
-        <v>0</v>
-      </c>
-      <c r="F86" s="3">
-        <f t="shared" si="84"/>
-        <v>0</v>
+      <c r="E86" s="3" t="str">
+        <f t="shared" ref="E86:F86" si="85">E176</f>
+        <v>HD66 .A383 1997 v.4</v>
+      </c>
+      <c r="F86" s="3" t="str">
+        <f t="shared" si="85"/>
+        <v>HD75 .I57 2006</v>
       </c>
       <c r="G86" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5509,8 +5770,8 @@
         <v>187</v>
       </c>
       <c r="I86" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -5527,13 +5788,13 @@
       <c r="D87" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E87" s="3">
-        <f t="shared" ref="E87:F87" si="85">E177</f>
-        <v>0</v>
-      </c>
-      <c r="F87" s="3">
-        <f t="shared" si="85"/>
-        <v>0</v>
+      <c r="E87" s="3" t="str">
+        <f t="shared" ref="E87:F87" si="86">E177</f>
+        <v>HD75 .K46 2011</v>
+      </c>
+      <c r="F87" s="3" t="str">
+        <f t="shared" si="86"/>
+        <v>HD2385 .I5 W48 2004</v>
       </c>
       <c r="G87" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5543,8 +5804,8 @@
         <v>187</v>
       </c>
       <c r="I87" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -5561,13 +5822,13 @@
       <c r="D88" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E88" s="3">
-        <f t="shared" ref="E88:F88" si="86">E178</f>
-        <v>0</v>
-      </c>
-      <c r="F88" s="3">
-        <f t="shared" si="86"/>
-        <v>0</v>
+      <c r="E88" s="3" t="str">
+        <f t="shared" ref="E88:F88" si="87">E178</f>
+        <v>HD2721 .M286 2008</v>
+      </c>
+      <c r="F88" s="3" t="str">
+        <f t="shared" si="87"/>
+        <v>HD3616 .E184 A24 1990</v>
       </c>
       <c r="G88" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5577,8 +5838,8 @@
         <v>187</v>
       </c>
       <c r="I88" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -5595,13 +5856,13 @@
       <c r="D89" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E89" s="3">
-        <f t="shared" ref="E89:F89" si="87">E179</f>
-        <v>0</v>
-      </c>
-      <c r="F89" s="3">
-        <f t="shared" si="87"/>
-        <v>0</v>
+      <c r="E89" s="3" t="str">
+        <f t="shared" ref="E89:F89" si="88">E179</f>
+        <v>HD3616 .E8 K37 1985</v>
+      </c>
+      <c r="F89" s="3" t="str">
+        <f t="shared" si="88"/>
+        <v>HD7096 .J3 E26 2004</v>
       </c>
       <c r="G89" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5611,8 +5872,8 @@
         <v>187</v>
       </c>
       <c r="I89" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -5629,13 +5890,13 @@
       <c r="D90" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E90" s="3">
-        <f t="shared" ref="E90:F90" si="88">E180</f>
-        <v>0</v>
-      </c>
-      <c r="F90" s="3">
-        <f t="shared" si="88"/>
-        <v>0</v>
+      <c r="E90" s="3" t="str">
+        <f t="shared" ref="E90:F90" si="89">E180</f>
+        <v>HD7103.65 .S55 F55 2017</v>
+      </c>
+      <c r="F90" s="3" t="str">
+        <f t="shared" si="89"/>
+        <v>HD9696.8 .U63 N745 2004</v>
       </c>
       <c r="G90" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5645,8 +5906,8 @@
         <v>187</v>
       </c>
       <c r="I90" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -5663,13 +5924,13 @@
       <c r="D91" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E91" s="3">
-        <f t="shared" ref="E91:F91" si="89">E181</f>
-        <v>0</v>
-      </c>
-      <c r="F91" s="3">
-        <f t="shared" si="89"/>
-        <v>0</v>
+      <c r="E91" s="3" t="str">
+        <f t="shared" ref="E91:F91" si="90">E181</f>
+        <v>HD9696.8 .U64 B73 2011</v>
+      </c>
+      <c r="F91" s="3" t="str">
+        <f t="shared" si="90"/>
+        <v>HE9897.8 .P52 1989</v>
       </c>
       <c r="G91" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
@@ -5679,8 +5940,8 @@
         <v>187</v>
       </c>
       <c r="I91" s="4" t="b">
-        <f t="shared" si="78"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -7123,8 +7384,12 @@
       <c r="D138" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E138" s="3"/>
-      <c r="F138" s="3"/>
+      <c r="E138" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>423</v>
+      </c>
       <c r="G138" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b1_a.png</v>
@@ -7133,7 +7398,7 @@
         <v>187</v>
       </c>
       <c r="I138" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -7150,8 +7415,12 @@
       <c r="D139" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E139" s="3"/>
-      <c r="F139" s="3"/>
+      <c r="E139" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>425</v>
+      </c>
       <c r="G139" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b1_b.png</v>
@@ -7160,7 +7429,7 @@
         <v>187</v>
       </c>
       <c r="I139" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -7177,8 +7446,12 @@
       <c r="D140" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E140" s="3"/>
-      <c r="F140" s="3"/>
+      <c r="E140" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>427</v>
+      </c>
       <c r="G140" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b2_a.png</v>
@@ -7187,7 +7460,7 @@
         <v>187</v>
       </c>
       <c r="I140" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -7204,8 +7477,12 @@
       <c r="D141" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E141" s="3"/>
-      <c r="F141" s="3"/>
+      <c r="E141" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="G141" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b2_b.png</v>
@@ -7214,7 +7491,7 @@
         <v>187</v>
       </c>
       <c r="I141" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -7231,8 +7508,12 @@
       <c r="D142" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E142" s="3"/>
-      <c r="F142" s="3"/>
+      <c r="E142" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>431</v>
+      </c>
       <c r="G142" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b3_a.png</v>
@@ -7241,7 +7522,7 @@
         <v>187</v>
       </c>
       <c r="I142" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -7258,8 +7539,12 @@
       <c r="D143" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E143" s="3"/>
-      <c r="F143" s="3"/>
+      <c r="E143" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>433</v>
+      </c>
       <c r="G143" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b3_b.png</v>
@@ -7268,7 +7553,7 @@
         <v>187</v>
       </c>
       <c r="I143" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -7285,8 +7570,12 @@
       <c r="D144" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
+      <c r="E144" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>509</v>
+      </c>
       <c r="G144" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b4_a.png</v>
@@ -7295,7 +7584,7 @@
         <v>187</v>
       </c>
       <c r="I144" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -7312,8 +7601,12 @@
       <c r="D145" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E145" s="3"/>
-      <c r="F145" s="3"/>
+      <c r="E145" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>436</v>
+      </c>
       <c r="G145" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b4_b.png</v>
@@ -7322,7 +7615,7 @@
         <v>187</v>
       </c>
       <c r="I145" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -7339,8 +7632,12 @@
       <c r="D146" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E146" s="3"/>
-      <c r="F146" s="3"/>
+      <c r="E146" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>438</v>
+      </c>
       <c r="G146" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b5_a.png</v>
@@ -7349,7 +7646,7 @@
         <v>187</v>
       </c>
       <c r="I146" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -7366,8 +7663,12 @@
       <c r="D147" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E147" s="3"/>
-      <c r="F147" s="3"/>
+      <c r="E147" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="F147" s="6" t="s">
+        <v>440</v>
+      </c>
       <c r="G147" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b5_b.png</v>
@@ -7376,7 +7677,7 @@
         <v>187</v>
       </c>
       <c r="I147" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -7393,8 +7694,12 @@
       <c r="D148" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E148" s="3"/>
-      <c r="F148" s="3"/>
+      <c r="E148" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>442</v>
+      </c>
       <c r="G148" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b6_a.png</v>
@@ -7403,7 +7708,7 @@
         <v>187</v>
       </c>
       <c r="I148" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -7420,8 +7725,12 @@
       <c r="D149" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
+      <c r="E149" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="G149" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b6_b.png</v>
@@ -7430,7 +7739,7 @@
         <v>187</v>
       </c>
       <c r="I149" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -7447,8 +7756,12 @@
       <c r="D150" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
+      <c r="E150" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>446</v>
+      </c>
       <c r="G150" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b7_a.png</v>
@@ -7457,7 +7770,7 @@
         <v>187</v>
       </c>
       <c r="I150" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -7474,8 +7787,12 @@
       <c r="D151" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
+      <c r="E151" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="F151" s="6" t="s">
+        <v>448</v>
+      </c>
       <c r="G151" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b7_b.png</v>
@@ -7484,7 +7801,7 @@
         <v>187</v>
       </c>
       <c r="I151" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -7501,8 +7818,12 @@
       <c r="D152" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E152" s="3"/>
-      <c r="F152" s="3"/>
+      <c r="E152" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>450</v>
+      </c>
       <c r="G152" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b8_a.png</v>
@@ -7511,7 +7832,7 @@
         <v>187</v>
       </c>
       <c r="I152" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -7528,8 +7849,12 @@
       <c r="D153" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E153" s="3"/>
-      <c r="F153" s="3"/>
+      <c r="E153" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>452</v>
+      </c>
       <c r="G153" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b8_b.png</v>
@@ -7538,7 +7863,7 @@
         <v>187</v>
       </c>
       <c r="I153" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -7555,8 +7880,12 @@
       <c r="D154" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
+      <c r="E154" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="F154" s="6" t="s">
+        <v>454</v>
+      </c>
       <c r="G154" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b9_a.png</v>
@@ -7565,7 +7894,7 @@
         <v>187</v>
       </c>
       <c r="I154" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -7582,8 +7911,12 @@
       <c r="D155" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E155" s="3"/>
-      <c r="F155" s="3"/>
+      <c r="E155" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>456</v>
+      </c>
       <c r="G155" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b9_b.png</v>
@@ -7592,7 +7925,7 @@
         <v>187</v>
       </c>
       <c r="I155" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -7609,8 +7942,12 @@
       <c r="D156" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
+      <c r="E156" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>458</v>
+      </c>
       <c r="G156" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b10_a.png</v>
@@ -7619,7 +7956,7 @@
         <v>187</v>
       </c>
       <c r="I156" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -7636,8 +7973,12 @@
       <c r="D157" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
+      <c r="E157" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="F157" s="6" t="s">
+        <v>460</v>
+      </c>
       <c r="G157" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b10_b.png</v>
@@ -7646,7 +7987,7 @@
         <v>187</v>
       </c>
       <c r="I157" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -7663,8 +8004,12 @@
       <c r="D158" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
+      <c r="E158" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>462</v>
+      </c>
       <c r="G158" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b11_a.png</v>
@@ -7673,7 +8018,7 @@
         <v>187</v>
       </c>
       <c r="I158" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -7690,8 +8035,12 @@
       <c r="D159" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E159" s="3"/>
-      <c r="F159" s="3"/>
+      <c r="E159" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>464</v>
+      </c>
       <c r="G159" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b11_b.png</v>
@@ -7700,7 +8049,7 @@
         <v>187</v>
       </c>
       <c r="I159" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -7717,8 +8066,12 @@
       <c r="D160" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
+      <c r="E160" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="F160" s="6" t="s">
+        <v>466</v>
+      </c>
       <c r="G160" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b12_a.png</v>
@@ -7727,7 +8080,7 @@
         <v>187</v>
       </c>
       <c r="I160" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -7744,8 +8097,12 @@
       <c r="D161" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
+      <c r="E161" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="F161" s="6" t="s">
+        <v>467</v>
+      </c>
       <c r="G161" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b12_b.png</v>
@@ -7754,7 +8111,7 @@
         <v>187</v>
       </c>
       <c r="I161" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -7771,8 +8128,12 @@
       <c r="D162" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
+      <c r="E162" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>469</v>
+      </c>
       <c r="G162" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b13_a.png</v>
@@ -7781,7 +8142,7 @@
         <v>187</v>
       </c>
       <c r="I162" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -7798,8 +8159,12 @@
       <c r="D163" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
+      <c r="E163" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>471</v>
+      </c>
       <c r="G163" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b13_b.png</v>
@@ -7808,7 +8173,7 @@
         <v>187</v>
       </c>
       <c r="I163" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -7825,8 +8190,12 @@
       <c r="D164" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
+      <c r="E164" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>473</v>
+      </c>
       <c r="G164" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b14_a.png</v>
@@ -7835,7 +8204,7 @@
         <v>187</v>
       </c>
       <c r="I164" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -7852,8 +8221,12 @@
       <c r="D165" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
+      <c r="E165" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="F165" s="6" t="s">
+        <v>475</v>
+      </c>
       <c r="G165" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b14_b.png</v>
@@ -7862,7 +8235,7 @@
         <v>187</v>
       </c>
       <c r="I165" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -7879,8 +8252,12 @@
       <c r="D166" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
+      <c r="E166" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="F166" s="6" t="s">
+        <v>477</v>
+      </c>
       <c r="G166" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b15_a.png</v>
@@ -7889,7 +8266,7 @@
         <v>187</v>
       </c>
       <c r="I166" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -7906,8 +8283,12 @@
       <c r="D167" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E167" s="3"/>
-      <c r="F167" s="3"/>
+      <c r="E167" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>479</v>
+      </c>
       <c r="G167" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b15_b.png</v>
@@ -7916,7 +8297,7 @@
         <v>187</v>
       </c>
       <c r="I167" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -7933,8 +8314,12 @@
       <c r="D168" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
+      <c r="E168" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>481</v>
+      </c>
       <c r="G168" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b16_a.png</v>
@@ -7943,7 +8328,7 @@
         <v>187</v>
       </c>
       <c r="I168" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -7960,8 +8345,12 @@
       <c r="D169" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E169" s="3"/>
-      <c r="F169" s="3"/>
+      <c r="E169" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="F169" s="6" t="s">
+        <v>483</v>
+      </c>
       <c r="G169" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b16_b.png</v>
@@ -7970,7 +8359,7 @@
         <v>187</v>
       </c>
       <c r="I169" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -7987,8 +8376,12 @@
       <c r="D170" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
+      <c r="E170" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F170" s="6" t="s">
+        <v>485</v>
+      </c>
       <c r="G170" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b17_a.png</v>
@@ -7997,7 +8390,7 @@
         <v>187</v>
       </c>
       <c r="I170" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -8014,8 +8407,12 @@
       <c r="D171" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E171" s="3"/>
-      <c r="F171" s="3"/>
+      <c r="E171" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="F171" s="6" t="s">
+        <v>487</v>
+      </c>
       <c r="G171" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b17_b.png</v>
@@ -8024,7 +8421,7 @@
         <v>187</v>
       </c>
       <c r="I171" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -8041,8 +8438,12 @@
       <c r="D172" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
+      <c r="E172" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="F172" s="6" t="s">
+        <v>489</v>
+      </c>
       <c r="G172" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b18_a.png</v>
@@ -8051,7 +8452,7 @@
         <v>187</v>
       </c>
       <c r="I172" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -8068,8 +8469,12 @@
       <c r="D173" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E173" s="3"/>
-      <c r="F173" s="3"/>
+      <c r="E173" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="F173" s="6" t="s">
+        <v>491</v>
+      </c>
       <c r="G173" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b18_b.png</v>
@@ -8078,7 +8483,7 @@
         <v>187</v>
       </c>
       <c r="I173" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -8095,8 +8500,12 @@
       <c r="D174" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E174" s="3"/>
-      <c r="F174" s="3"/>
+      <c r="E174" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>492</v>
+      </c>
       <c r="G174" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b19_a.png</v>
@@ -8105,7 +8514,7 @@
         <v>187</v>
       </c>
       <c r="I174" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -8122,8 +8531,12 @@
       <c r="D175" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E175" s="3"/>
-      <c r="F175" s="3"/>
+      <c r="E175" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="F175" s="6" t="s">
+        <v>494</v>
+      </c>
       <c r="G175" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b19_b.png</v>
@@ -8132,7 +8545,7 @@
         <v>187</v>
       </c>
       <c r="I175" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -8149,8 +8562,12 @@
       <c r="D176" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E176" s="3"/>
-      <c r="F176" s="3"/>
+      <c r="E176" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>496</v>
+      </c>
       <c r="G176" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b20_a.png</v>
@@ -8159,7 +8576,7 @@
         <v>187</v>
       </c>
       <c r="I176" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -8176,8 +8593,12 @@
       <c r="D177" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E177" s="3"/>
-      <c r="F177" s="3"/>
+      <c r="E177" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>498</v>
+      </c>
       <c r="G177" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b20_b.png</v>
@@ -8186,7 +8607,7 @@
         <v>187</v>
       </c>
       <c r="I177" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -8203,8 +8624,12 @@
       <c r="D178" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E178" s="3"/>
-      <c r="F178" s="3"/>
+      <c r="E178" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="F178" s="6" t="s">
+        <v>500</v>
+      </c>
       <c r="G178" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b21_a.png</v>
@@ -8213,7 +8638,7 @@
         <v>187</v>
       </c>
       <c r="I178" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -8230,8 +8655,12 @@
       <c r="D179" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E179" s="3"/>
-      <c r="F179" s="3"/>
+      <c r="E179" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>502</v>
+      </c>
       <c r="G179" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b21_b.png</v>
@@ -8240,7 +8669,7 @@
         <v>187</v>
       </c>
       <c r="I179" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -8257,8 +8686,12 @@
       <c r="D180" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E180" s="3"/>
-      <c r="F180" s="3"/>
+      <c r="E180" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="F180" s="6" t="s">
+        <v>504</v>
+      </c>
       <c r="G180" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b22_a.png</v>
@@ -8267,7 +8700,7 @@
         <v>187</v>
       </c>
       <c r="I180" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -8284,8 +8717,12 @@
       <c r="D181" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
+      <c r="E181" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="F181" s="6" t="s">
+        <v>506</v>
+      </c>
       <c r="G181" s="3" t="str">
         <f xml:space="preserve"> "main_l4_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l4_b22_b.png</v>
@@ -8294,7 +8731,7 @@
         <v>187</v>
       </c>
       <c r="I181" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -8311,8 +8748,8 @@
       <c r="D182" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E182" s="3"/>
-      <c r="F182" s="3"/>
+      <c r="E182" s="6"/>
+      <c r="F182" s="6"/>
       <c r="G182" s="3" t="str">
         <f xml:space="preserve"> "main_l3_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l3_j1_a.png</v>

</xml_diff>

<commit_message>
Update maps for MAIN L3 journals
</commit_message>
<xml_diff>
--- a/utils/datastore_from_xlsx_sample_input.xlsx
+++ b/utils/datastore_from_xlsx_sample_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16890" windowHeight="6810" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16890" windowHeight="6810"/>
   </bookViews>
   <sheets>
     <sheet name="Libraries" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="519">
   <si>
     <t>_id</t>
   </si>
@@ -1556,6 +1556,33 @@
   </si>
   <si>
     <t>BF531 .O94 2009</t>
+  </si>
+  <si>
+    <t>B1 .J6</t>
+  </si>
+  <si>
+    <t>HB1 .J642</t>
+  </si>
+  <si>
+    <t>HB1 .M27</t>
+  </si>
+  <si>
+    <t>HB99.5 .J68</t>
+  </si>
+  <si>
+    <t>HD61 .J67</t>
+  </si>
+  <si>
+    <t>HD87 .A44</t>
+  </si>
+  <si>
+    <t>HF5601 .J73</t>
+  </si>
+  <si>
+    <t>HF5601 .M39</t>
+  </si>
+  <si>
+    <t>T1 .S5</t>
   </si>
 </sst>
 </file>
@@ -1858,8 +1885,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="datastore__4" displayName="datastore__4" ref="A1:I277" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I277"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="datastore__4" displayName="datastore__4" ref="A1:I278" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I278"/>
   <tableColumns count="9">
     <tableColumn id="18" name="_id" dataDxfId="8"/>
     <tableColumn id="19" name="doctype" dataDxfId="7"/>
@@ -2140,7 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2234,7 +2261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2436,7 +2463,7 @@
         <v>36</v>
       </c>
       <c r="F9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2832,7 +2859,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I277"/>
+  <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5158,7 +5185,7 @@
         <v>187</v>
       </c>
       <c r="I68" s="4" t="b">
-        <f t="shared" ref="I67:I78" si="66">I158</f>
+        <f t="shared" ref="I68:I78" si="66">I158</f>
         <v>1</v>
       </c>
     </row>
@@ -8748,8 +8775,12 @@
       <c r="D182" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E182" s="6"/>
-      <c r="F182" s="6"/>
+      <c r="E182" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="F182" s="6" t="s">
+        <v>511</v>
+      </c>
       <c r="G182" s="3" t="str">
         <f xml:space="preserve"> "main_l3_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l3_j1_a.png</v>
@@ -8758,7 +8789,7 @@
         <v>187</v>
       </c>
       <c r="I182" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -8775,8 +8806,12 @@
       <c r="D183" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E183" s="3"/>
-      <c r="F183" s="3"/>
+      <c r="E183" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="F183" s="6" t="s">
+        <v>512</v>
+      </c>
       <c r="G183" s="3" t="str">
         <f xml:space="preserve"> "main_l3_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l3_j1_b.png</v>
@@ -8785,40 +8820,44 @@
         <v>187</v>
       </c>
       <c r="I183" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>MAIN JournalL3 J2-A</v>
+        <v>MAIN JournalL3 J1-C</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C184" s="3" t="s">
+      <c r="C184" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D184" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E184" s="3"/>
-      <c r="F184" s="3"/>
+      <c r="D184" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="F184" s="6" t="s">
+        <v>514</v>
+      </c>
       <c r="G184" s="3" t="str">
         <f xml:space="preserve"> "main_l3_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
-        <v>main_l3_j2_a.png</v>
+        <v>main_l3_j1_c.png</v>
       </c>
       <c r="H184" s="3" t="s">
         <v>187</v>
       </c>
       <c r="I184" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>MAIN JournalL3 J2-B</v>
+        <v>MAIN JournalL3 J2-A</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>74</v>
@@ -8827,447 +8866,452 @@
         <v>34</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="E185" s="3"/>
-      <c r="F185" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="F185" s="6" t="s">
+        <v>516</v>
+      </c>
       <c r="G185" s="3" t="str">
         <f xml:space="preserve"> "main_l3_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
-        <v>main_l3_j2_b.png</v>
+        <v>main_l3_j2_a.png</v>
       </c>
       <c r="H185" s="3" t="s">
         <v>187</v>
       </c>
       <c r="I185" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
+        <v>MAIN JournalL3 J2-B</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="F186" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="G186" s="3" t="str">
+        <f xml:space="preserve"> "main_l3_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
+        <v>main_l3_j2_b.png</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I186" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="str">
+        <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN Lifestyle L-A</v>
       </c>
-      <c r="B186" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C186" s="3" t="s">
+      <c r="B187" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C187" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D186" s="3" t="s">
+      <c r="D187" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E186" s="3" t="s">
+      <c r="E187" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F186" s="3" t="s">
+      <c r="F187" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="G186" s="3" t="str">
+      <c r="G187" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_l_a.png</v>
       </c>
-      <c r="H186" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I186" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="str">
+      <c r="H187" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I187" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN Lifestyle L-B</v>
       </c>
-      <c r="B187" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C187" s="3" t="s">
+      <c r="B188" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C188" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D187" s="3" t="s">
+      <c r="D188" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E187" s="3" t="s">
+      <c r="E188" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F187" s="3" t="s">
+      <c r="F188" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="G187" s="3" t="str">
+      <c r="G188" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_l_b.png</v>
       </c>
-      <c r="H187" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I187" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="3" t="str">
+      <c r="H188" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I188" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN Lifestyle L-C</v>
       </c>
-      <c r="B188" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C188" s="3" t="s">
+      <c r="B189" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D188" s="3" t="s">
+      <c r="D189" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E188" s="3" t="s">
+      <c r="E189" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="F188" s="3" t="s">
+      <c r="F189" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="G188" s="3" t="str">
+      <c r="G189" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_l_c.png</v>
       </c>
-      <c r="H188" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I188" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="3" t="str">
+      <c r="H189" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I189" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN MediaLvl2 M-A</v>
       </c>
-      <c r="B189" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C189" s="3" t="s">
+      <c r="B190" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C190" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D189" s="3" t="s">
+      <c r="D190" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E189" s="3" t="s">
+      <c r="E190" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F189" s="3" t="s">
+      <c r="F190" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G189" s="3" t="str">
+      <c r="G190" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_m_a.png</v>
       </c>
-      <c r="H189" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I189" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="3" t="str">
+      <c r="H190" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I190" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN MediaLvl2 M-B</v>
       </c>
-      <c r="B190" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C190" s="3" t="s">
+      <c r="B191" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C191" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D191" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E190" s="3" t="s">
+      <c r="E191" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="F190" s="3" t="s">
+      <c r="F191" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G190" s="3" t="str">
+      <c r="G191" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_m_b.png</v>
       </c>
-      <c r="H190" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I190" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="str">
+      <c r="H191" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I191" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN NewsLvl2 NM1-A</v>
       </c>
-      <c r="B191" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C191" s="3" t="s">
+      <c r="B192" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C192" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D191" s="3" t="s">
+      <c r="D192" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E191" s="3" t="s">
+      <c r="E192" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F191" s="3" t="s">
+      <c r="F192" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G191" s="3" t="str">
+      <c r="G192" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_nm1_a.png</v>
       </c>
-      <c r="H191" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I191" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="str">
+      <c r="H192" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I192" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN NewsLvl2 NM1-B</v>
       </c>
-      <c r="B192" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C192" s="3" t="s">
+      <c r="B193" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C193" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D192" s="3" t="s">
+      <c r="D193" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E192" s="3" t="s">
+      <c r="E193" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F192" s="3" t="s">
+      <c r="F193" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="G192" s="3" t="str">
+      <c r="G193" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_nm1_b.png</v>
       </c>
-      <c r="H192" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I192" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="str">
+      <c r="H193" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I193" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN NewsLvl2 NM2</v>
       </c>
-      <c r="B193" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C193" s="3" t="s">
+      <c r="B194" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C194" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D193" s="3" t="s">
+      <c r="D194" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E193" s="3" t="s">
+      <c r="E194" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F193" s="3" t="s">
+      <c r="F194" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G193" s="3" t="str">
+      <c r="G194" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_nm2.png</v>
       </c>
-      <c r="H193" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I193" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="3" t="str">
+      <c r="H194" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I194" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN CRMedia CRM</v>
       </c>
-      <c r="B194" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C194" s="3" t="s">
+      <c r="B195" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C195" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D194" s="3" t="s">
+      <c r="D195" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E194" s="3" t="s">
+      <c r="E195" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F194" s="3" t="s">
+      <c r="F195" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G194" s="3" t="str">
+      <c r="G195" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_crm.png</v>
       </c>
-      <c r="H194" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I194" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="str">
+      <c r="H195" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I195" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN CR3H CR1-A</v>
       </c>
-      <c r="B195" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C195" s="3" t="s">
+      <c r="B196" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C196" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D195" s="3" t="s">
+      <c r="D196" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E195" s="3" t="s">
+      <c r="E196" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F195" s="3" t="s">
+      <c r="F196" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G195" s="3" t="str">
+      <c r="G196" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_cr1_a.png</v>
       </c>
-      <c r="H195" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I195" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A196" s="3" t="str">
+      <c r="H196" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I196" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN CR3H CR1-B</v>
       </c>
-      <c r="B196" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C196" s="3" t="s">
+      <c r="B197" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C197" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D196" s="3" t="s">
+      <c r="D197" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E196" s="3" t="s">
+      <c r="E197" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F196" s="3" t="s">
+      <c r="F197" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="G196" s="3" t="str">
+      <c r="G197" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_cr1_b.png</v>
       </c>
-      <c r="H196" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I196" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A197" s="3" t="str">
+      <c r="H197" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I197" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN CR3H CR2-A</v>
       </c>
-      <c r="B197" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C197" s="3" t="s">
+      <c r="B198" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C198" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D197" s="3" t="s">
+      <c r="D198" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E197" s="3" t="s">
+      <c r="E198" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F197" s="3" t="s">
+      <c r="F198" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G197" s="3" t="str">
+      <c r="G198" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_cr2_a.png</v>
       </c>
-      <c r="H197" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I197" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A198" s="3" t="str">
+      <c r="H198" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I198" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
         <v>MAIN CR3H CR2-B</v>
       </c>
-      <c r="B198" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C198" s="3" t="s">
+      <c r="B199" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C199" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D198" s="3" t="s">
+      <c r="D199" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E198" s="3" t="s">
+      <c r="E199" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F198" s="3" t="s">
+      <c r="F199" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G198" s="3" t="str">
+      <c r="G199" s="3" t="str">
         <f xml:space="preserve"> "main_l2_" &amp; LOWER(SUBSTITUTE(datastore__4[[#This Row],[code]],"-","_")) &amp; ".png"</f>
         <v>main_l2_cr2_b.png</v>
       </c>
-      <c r="H198" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I198" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="str">
-        <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B1-A</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D199" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E199" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F199" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G199" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="H199" s="3" t="s">
         <v>187</v>
       </c>
@@ -9278,7 +9322,7 @@
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B1-B</v>
+        <v>KGC 3DaysL4 B1-A</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>74</v>
@@ -9287,16 +9331,16 @@
         <v>56</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>230</v>
+        <v>99</v>
       </c>
       <c r="F200" s="3" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H200" s="3" t="s">
         <v>187</v>
@@ -9308,7 +9352,7 @@
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B2-A</v>
+        <v>KGC 3DaysL4 B1-B</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>74</v>
@@ -9317,16 +9361,16 @@
         <v>56</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="F201" s="3" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>187</v>
@@ -9338,7 +9382,7 @@
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B2-B</v>
+        <v>KGC 3DaysL4 B2-A</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>74</v>
@@ -9347,16 +9391,16 @@
         <v>56</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="F202" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>187</v>
@@ -9368,7 +9412,7 @@
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B3-A</v>
+        <v>KGC 3DaysL4 B2-B</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>74</v>
@@ -9377,16 +9421,16 @@
         <v>56</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E203" s="3" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="F203" s="3" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H203" s="3" t="s">
         <v>187</v>
@@ -9398,7 +9442,7 @@
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B3-B</v>
+        <v>KGC 3DaysL4 B3-A</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>74</v>
@@ -9407,16 +9451,16 @@
         <v>56</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>187</v>
@@ -9428,7 +9472,7 @@
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B4-A</v>
+        <v>KGC 3DaysL4 B3-B</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>74</v>
@@ -9437,16 +9481,16 @@
         <v>56</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H205" s="3" t="s">
         <v>187</v>
@@ -9458,7 +9502,7 @@
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B4-B</v>
+        <v>KGC 3DaysL4 B4-A</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>74</v>
@@ -9467,16 +9511,16 @@
         <v>56</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>187</v>
@@ -9488,7 +9532,7 @@
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B5-A</v>
+        <v>KGC 3DaysL4 B4-B</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>74</v>
@@ -9497,16 +9541,16 @@
         <v>56</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="G207" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H207" s="3" t="s">
         <v>187</v>
@@ -9518,7 +9562,7 @@
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B5-B</v>
+        <v>KGC 3DaysL4 B5-A</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>74</v>
@@ -9527,16 +9571,16 @@
         <v>56</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>320</v>
+        <v>246</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>187</v>
@@ -9548,7 +9592,7 @@
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B6-A</v>
+        <v>KGC 3DaysL4 B5-B</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>74</v>
@@ -9557,16 +9601,16 @@
         <v>56</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>220</v>
+        <v>320</v>
       </c>
       <c r="F209" s="3" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H209" s="3" t="s">
         <v>187</v>
@@ -9578,7 +9622,7 @@
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B6-B</v>
+        <v>KGC 3DaysL4 B6-A</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>74</v>
@@ -9587,16 +9631,16 @@
         <v>56</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H210" s="3" t="s">
         <v>187</v>
@@ -9608,7 +9652,7 @@
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B7-A</v>
+        <v>KGC 3DaysL4 B6-B</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>74</v>
@@ -9617,16 +9661,16 @@
         <v>56</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H211" s="3" t="s">
         <v>187</v>
@@ -9638,7 +9682,7 @@
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B7-B</v>
+        <v>KGC 3DaysL4 B7-A</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>74</v>
@@ -9647,16 +9691,16 @@
         <v>56</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="F212" s="3" t="s">
-        <v>219</v>
+        <v>259</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H212" s="3" t="s">
         <v>187</v>
@@ -9668,7 +9712,7 @@
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B8-A</v>
+        <v>KGC 3DaysL4 B7-B</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>74</v>
@@ -9677,16 +9721,16 @@
         <v>56</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F213" s="3" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>187</v>
@@ -9698,7 +9742,7 @@
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B8-B</v>
+        <v>KGC 3DaysL4 B8-A</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>74</v>
@@ -9707,16 +9751,16 @@
         <v>56</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="F214" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G214" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H214" s="3" t="s">
         <v>187</v>
@@ -9728,7 +9772,7 @@
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B9-A</v>
+        <v>KGC 3DaysL4 B8-B</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>74</v>
@@ -9737,16 +9781,16 @@
         <v>56</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E215" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="F215" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>187</v>
@@ -9758,7 +9802,7 @@
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B9-B</v>
+        <v>KGC 3DaysL4 B9-A</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>74</v>
@@ -9767,16 +9811,16 @@
         <v>56</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F216" s="3" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H216" s="3" t="s">
         <v>187</v>
@@ -9788,7 +9832,7 @@
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B10-A</v>
+        <v>KGC 3DaysL4 B9-B</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>74</v>
@@ -9797,16 +9841,16 @@
         <v>56</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="F217" s="3" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H217" s="3" t="s">
         <v>187</v>
@@ -9818,7 +9862,7 @@
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B10-B</v>
+        <v>KGC 3DaysL4 B10-A</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>74</v>
@@ -9827,16 +9871,16 @@
         <v>56</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F218" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>187</v>
@@ -9848,7 +9892,7 @@
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B11-A</v>
+        <v>KGC 3DaysL4 B10-B</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>74</v>
@@ -9857,16 +9901,16 @@
         <v>56</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="F219" s="3" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="G219" s="3" t="s">
-        <v>203</v>
+        <v>138</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>187</v>
@@ -9878,7 +9922,7 @@
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B11-B</v>
+        <v>KGC 3DaysL4 B11-A</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>74</v>
@@ -9887,16 +9931,16 @@
         <v>56</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>193</v>
+        <v>239</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>187</v>
@@ -9908,7 +9952,7 @@
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B11-C</v>
+        <v>KGC 3DaysL4 B11-B</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>74</v>
@@ -9917,16 +9961,16 @@
         <v>56</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="F221" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="G221" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H221" s="3" t="s">
         <v>187</v>
@@ -9938,7 +9982,7 @@
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B12-A</v>
+        <v>KGC 3DaysL4 B11-C</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>74</v>
@@ -9947,16 +9991,16 @@
         <v>56</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="F222" s="3" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H222" s="3" t="s">
         <v>187</v>
@@ -9968,7 +10012,7 @@
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B12-B</v>
+        <v>KGC 3DaysL4 B12-A</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>74</v>
@@ -9977,16 +10021,16 @@
         <v>56</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="F223" s="3" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H223" s="3" t="s">
         <v>187</v>
@@ -9998,7 +10042,7 @@
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B13-A</v>
+        <v>KGC 3DaysL4 B12-B</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>74</v>
@@ -10007,16 +10051,16 @@
         <v>56</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H224" s="3" t="s">
         <v>187</v>
@@ -10028,7 +10072,7 @@
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC 3DaysL4 B13-B</v>
+        <v>KGC 3DaysL4 B13-A</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>74</v>
@@ -10037,16 +10081,16 @@
         <v>56</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G225" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H225" s="3" t="s">
         <v>187</v>
@@ -10058,25 +10102,25 @@
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B1-A</v>
+        <v>KGC 3DaysL4 B13-B</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>99</v>
+        <v>213</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="G226" s="3" t="s">
-        <v>100</v>
+        <v>209</v>
       </c>
       <c r="H226" s="3" t="s">
         <v>187</v>
@@ -10088,7 +10132,7 @@
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B1-B</v>
+        <v>KGC LendingL4 B1-A</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>74</v>
@@ -10097,16 +10141,16 @@
         <v>58</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>230</v>
+        <v>99</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
       <c r="G227" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H227" s="3" t="s">
         <v>187</v>
@@ -10118,7 +10162,7 @@
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B2-A</v>
+        <v>KGC LendingL4 B1-B</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>74</v>
@@ -10127,16 +10171,16 @@
         <v>58</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="G228" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H228" s="3" t="s">
         <v>187</v>
@@ -10148,7 +10192,7 @@
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B2-B</v>
+        <v>KGC LendingL4 B2-A</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>74</v>
@@ -10157,16 +10201,16 @@
         <v>58</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="F229" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H229" s="3" t="s">
         <v>187</v>
@@ -10178,7 +10222,7 @@
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B3-A</v>
+        <v>KGC LendingL4 B2-B</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>74</v>
@@ -10187,16 +10231,16 @@
         <v>58</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="F230" s="3" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="G230" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H230" s="3" t="s">
         <v>187</v>
@@ -10208,7 +10252,7 @@
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B3-B</v>
+        <v>KGC LendingL4 B3-A</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>74</v>
@@ -10217,16 +10261,16 @@
         <v>58</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="G231" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H231" s="3" t="s">
         <v>187</v>
@@ -10238,7 +10282,7 @@
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B4-A</v>
+        <v>KGC LendingL4 B3-B</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>74</v>
@@ -10247,16 +10291,16 @@
         <v>58</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H232" s="3" t="s">
         <v>187</v>
@@ -10268,7 +10312,7 @@
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B4-B</v>
+        <v>KGC LendingL4 B4-A</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>74</v>
@@ -10277,16 +10321,16 @@
         <v>58</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F233" s="3" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G233" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H233" s="3" t="s">
         <v>187</v>
@@ -10298,7 +10342,7 @@
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B5-A</v>
+        <v>KGC LendingL4 B4-B</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>74</v>
@@ -10307,16 +10351,16 @@
         <v>58</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H234" s="3" t="s">
         <v>187</v>
@@ -10328,7 +10372,7 @@
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B5-B</v>
+        <v>KGC LendingL4 B5-A</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>74</v>
@@ -10337,16 +10381,16 @@
         <v>58</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>320</v>
+        <v>246</v>
       </c>
       <c r="F235" s="3" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="G235" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H235" s="3" t="s">
         <v>187</v>
@@ -10358,7 +10402,7 @@
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B6-A</v>
+        <v>KGC LendingL4 B5-B</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>74</v>
@@ -10367,16 +10411,16 @@
         <v>58</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E236" s="3" t="s">
-        <v>220</v>
+        <v>320</v>
       </c>
       <c r="F236" s="3" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H236" s="3" t="s">
         <v>187</v>
@@ -10388,7 +10432,7 @@
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B6-B</v>
+        <v>KGC LendingL4 B6-A</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>74</v>
@@ -10397,16 +10441,16 @@
         <v>58</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E237" s="3" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="F237" s="3" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="G237" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H237" s="3" t="s">
         <v>187</v>
@@ -10418,7 +10462,7 @@
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B7-A</v>
+        <v>KGC LendingL4 B6-B</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>74</v>
@@ -10427,16 +10471,16 @@
         <v>58</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="F238" s="3" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="G238" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H238" s="3" t="s">
         <v>187</v>
@@ -10448,7 +10492,7 @@
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B7-B</v>
+        <v>KGC LendingL4 B7-A</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>74</v>
@@ -10457,16 +10501,16 @@
         <v>58</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>219</v>
+        <v>259</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H239" s="3" t="s">
         <v>187</v>
@@ -10478,7 +10522,7 @@
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B8-A</v>
+        <v>KGC LendingL4 B7-B</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>74</v>
@@ -10487,16 +10531,16 @@
         <v>58</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="G240" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H240" s="3" t="s">
         <v>187</v>
@@ -10508,7 +10552,7 @@
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B8-B</v>
+        <v>KGC LendingL4 B8-A</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>74</v>
@@ -10517,16 +10561,16 @@
         <v>58</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E241" s="3" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="F241" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G241" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H241" s="3" t="s">
         <v>187</v>
@@ -10538,7 +10582,7 @@
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B9-A</v>
+        <v>KGC LendingL4 B8-B</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>74</v>
@@ -10547,16 +10591,16 @@
         <v>58</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="F242" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G242" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H242" s="3" t="s">
         <v>187</v>
@@ -10568,7 +10612,7 @@
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B9-B</v>
+        <v>KGC LendingL4 B9-A</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>74</v>
@@ -10577,16 +10621,16 @@
         <v>58</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E243" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F243" s="3" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="G243" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H243" s="3" t="s">
         <v>187</v>
@@ -10598,7 +10642,7 @@
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B10-A</v>
+        <v>KGC LendingL4 B9-B</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>74</v>
@@ -10607,16 +10651,16 @@
         <v>58</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="F244" s="3" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="G244" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H244" s="3" t="s">
         <v>187</v>
@@ -10628,7 +10672,7 @@
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B10-B</v>
+        <v>KGC LendingL4 B10-A</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>74</v>
@@ -10637,16 +10681,16 @@
         <v>58</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F245" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G245" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H245" s="3" t="s">
         <v>187</v>
@@ -10658,7 +10702,7 @@
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B11-A</v>
+        <v>KGC LendingL4 B10-B</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>74</v>
@@ -10667,16 +10711,16 @@
         <v>58</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="G246" s="3" t="s">
-        <v>203</v>
+        <v>138</v>
       </c>
       <c r="H246" s="3" t="s">
         <v>187</v>
@@ -10688,7 +10732,7 @@
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B11-B</v>
+        <v>KGC LendingL4 B11-A</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>74</v>
@@ -10697,16 +10741,16 @@
         <v>58</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>193</v>
+        <v>239</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="G247" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H247" s="3" t="s">
         <v>187</v>
@@ -10718,7 +10762,7 @@
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B11-C</v>
+        <v>KGC LendingL4 B11-B</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>74</v>
@@ -10727,16 +10771,16 @@
         <v>58</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="E248" s="3" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="G248" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H248" s="3" t="s">
         <v>187</v>
@@ -10748,7 +10792,7 @@
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B12-A</v>
+        <v>KGC LendingL4 B11-C</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>74</v>
@@ -10757,16 +10801,16 @@
         <v>58</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="F249" s="3" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="G249" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H249" s="3" t="s">
         <v>187</v>
@@ -10778,7 +10822,7 @@
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B12-B</v>
+        <v>KGC LendingL4 B12-A</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>74</v>
@@ -10787,16 +10831,16 @@
         <v>58</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E250" s="3" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="F250" s="3" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H250" s="3" t="s">
         <v>187</v>
@@ -10808,7 +10852,7 @@
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B13-A</v>
+        <v>KGC LendingL4 B12-B</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>74</v>
@@ -10817,16 +10861,16 @@
         <v>58</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E251" s="3" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="F251" s="3" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H251" s="3" t="s">
         <v>187</v>
@@ -10838,7 +10882,7 @@
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC LendingL4 B13-B</v>
+        <v>KGC LendingL4 B13-A</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>74</v>
@@ -10847,16 +10891,16 @@
         <v>58</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="F252" s="3" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G252" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H252" s="3" t="s">
         <v>187</v>
@@ -10868,25 +10912,25 @@
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J1-A</v>
+        <v>KGC LendingL4 B13-B</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="E253" s="3" t="s">
-        <v>304</v>
+        <v>213</v>
       </c>
       <c r="F253" s="3" t="s">
-        <v>305</v>
+        <v>231</v>
       </c>
       <c r="G253" s="3" t="s">
-        <v>293</v>
+        <v>209</v>
       </c>
       <c r="H253" s="3" t="s">
         <v>187</v>
@@ -10898,7 +10942,7 @@
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J1-B</v>
+        <v>KGC JournalsL4 J1-A</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>74</v>
@@ -10907,16 +10951,16 @@
         <v>64</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E254" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F254" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G254" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H254" s="3" t="s">
         <v>187</v>
@@ -10928,7 +10972,7 @@
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J1-C</v>
+        <v>KGC JournalsL4 J1-B</v>
       </c>
       <c r="B255" s="3" t="s">
         <v>74</v>
@@ -10937,16 +10981,16 @@
         <v>64</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>285</v>
+        <v>154</v>
       </c>
       <c r="E255" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F255" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G255" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H255" s="3" t="s">
         <v>187</v>
@@ -10958,7 +11002,7 @@
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J1-D</v>
+        <v>KGC JournalsL4 J1-C</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>74</v>
@@ -10967,16 +11011,16 @@
         <v>64</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E256" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F256" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G256" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H256" s="3" t="s">
         <v>187</v>
@@ -10988,7 +11032,7 @@
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J2-A</v>
+        <v>KGC JournalsL4 J1-D</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>74</v>
@@ -10997,16 +11041,16 @@
         <v>64</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>155</v>
+        <v>286</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F257" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G257" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H257" s="3" t="s">
         <v>187</v>
@@ -11018,7 +11062,7 @@
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J2-B</v>
+        <v>KGC JournalsL4 J2-A</v>
       </c>
       <c r="B258" s="3" t="s">
         <v>74</v>
@@ -11027,16 +11071,16 @@
         <v>64</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>287</v>
+        <v>155</v>
       </c>
       <c r="E258" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F258" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G258" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H258" s="3" t="s">
         <v>187</v>
@@ -11048,7 +11092,7 @@
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J2-C</v>
+        <v>KGC JournalsL4 J2-B</v>
       </c>
       <c r="B259" s="3" t="s">
         <v>74</v>
@@ -11057,16 +11101,16 @@
         <v>64</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E259" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F259" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G259" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H259" s="3" t="s">
         <v>187</v>
@@ -11078,7 +11122,7 @@
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J2-D</v>
+        <v>KGC JournalsL4 J2-C</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>74</v>
@@ -11087,16 +11131,16 @@
         <v>64</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E260" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F260" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G260" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H260" s="3" t="s">
         <v>187</v>
@@ -11108,7 +11152,7 @@
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J3-A</v>
+        <v>KGC JournalsL4 J2-D</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>74</v>
@@ -11117,16 +11161,16 @@
         <v>64</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F261" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G261" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H261" s="3" t="s">
         <v>187</v>
@@ -11138,7 +11182,7 @@
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J3-B</v>
+        <v>KGC JournalsL4 J3-A</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>74</v>
@@ -11147,16 +11191,16 @@
         <v>64</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F262" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G262" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H262" s="3" t="s">
         <v>187</v>
@@ -11168,7 +11212,7 @@
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC JournalsL4 J3-C</v>
+        <v>KGC JournalsL4 J3-B</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>74</v>
@@ -11177,16 +11221,16 @@
         <v>64</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E263" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F263" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G263" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H263" s="3" t="s">
         <v>187</v>
@@ -11198,25 +11242,25 @@
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR1-A</v>
+        <v>KGC JournalsL4 J3-C</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="E264" s="3" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="F264" s="3" t="s">
-        <v>275</v>
+        <v>319</v>
       </c>
       <c r="G264" s="3" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="H264" s="3" t="s">
         <v>187</v>
@@ -11228,7 +11272,7 @@
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR1-B</v>
+        <v>KGC ReportL4 LR1-A</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>74</v>
@@ -11237,16 +11281,16 @@
         <v>67</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E265" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F265" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G265" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H265" s="3" t="s">
         <v>187</v>
@@ -11258,7 +11302,7 @@
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR1-C</v>
+        <v>KGC ReportL4 LR1-B</v>
       </c>
       <c r="B266" s="3" t="s">
         <v>74</v>
@@ -11267,16 +11311,16 @@
         <v>67</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E266" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F266" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G266" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H266" s="3" t="s">
         <v>187</v>
@@ -11288,7 +11332,7 @@
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR1-D</v>
+        <v>KGC ReportL4 LR1-C</v>
       </c>
       <c r="B267" s="3" t="s">
         <v>74</v>
@@ -11297,16 +11341,16 @@
         <v>67</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E267" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F267" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G267" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H267" s="3" t="s">
         <v>187</v>
@@ -11318,7 +11362,7 @@
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR2-A</v>
+        <v>KGC ReportL4 LR1-D</v>
       </c>
       <c r="B268" s="3" t="s">
         <v>74</v>
@@ -11327,16 +11371,16 @@
         <v>67</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E268" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F268" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G268" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H268" s="3" t="s">
         <v>187</v>
@@ -11348,7 +11392,7 @@
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR2-B</v>
+        <v>KGC ReportL4 LR2-A</v>
       </c>
       <c r="B269" s="3" t="s">
         <v>74</v>
@@ -11357,16 +11401,16 @@
         <v>67</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F269" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G269" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H269" s="3" t="s">
         <v>187</v>
@@ -11378,7 +11422,7 @@
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC ReportL4 LR2-C</v>
+        <v>KGC ReportL4 LR2-B</v>
       </c>
       <c r="B270" s="3" t="s">
         <v>74</v>
@@ -11387,16 +11431,16 @@
         <v>67</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E270" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F270" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G270" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H270" s="3" t="s">
         <v>187</v>
@@ -11408,25 +11452,25 @@
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR1</v>
+        <v>KGC ReportL4 LR2-C</v>
       </c>
       <c r="B271" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>139</v>
+        <v>266</v>
       </c>
       <c r="E271" s="3" t="s">
-        <v>140</v>
+        <v>283</v>
       </c>
       <c r="F271" s="3" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="G271" s="3" t="s">
-        <v>141</v>
+        <v>273</v>
       </c>
       <c r="H271" s="3" t="s">
         <v>187</v>
@@ -11438,7 +11482,7 @@
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR2-A</v>
+        <v>KGC CR3H CR1</v>
       </c>
       <c r="B272" s="3" t="s">
         <v>74</v>
@@ -11447,16 +11491,16 @@
         <v>72</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="E272" s="3" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="F272" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G272" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H272" s="3" t="s">
         <v>187</v>
@@ -11468,7 +11512,7 @@
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR2-B</v>
+        <v>KGC CR3H CR2-A</v>
       </c>
       <c r="B273" s="3" t="s">
         <v>74</v>
@@ -11477,16 +11521,16 @@
         <v>72</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E273" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F273" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G273" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H273" s="3" t="s">
         <v>187</v>
@@ -11498,7 +11542,7 @@
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR3-A</v>
+        <v>KGC CR3H CR2-B</v>
       </c>
       <c r="B274" s="3" t="s">
         <v>74</v>
@@ -11507,16 +11551,16 @@
         <v>72</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="E274" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F274" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G274" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H274" s="3" t="s">
         <v>187</v>
@@ -11528,7 +11572,7 @@
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR3-B</v>
+        <v>KGC CR3H CR3-A</v>
       </c>
       <c r="B275" s="3" t="s">
         <v>74</v>
@@ -11537,16 +11581,16 @@
         <v>72</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E275" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F275" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G275" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H275" s="3" t="s">
         <v>187</v>
@@ -11558,7 +11602,7 @@
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR4</v>
+        <v>KGC CR3H CR3-B</v>
       </c>
       <c r="B276" s="3" t="s">
         <v>74</v>
@@ -11567,16 +11611,16 @@
         <v>72</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E276" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F276" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G276" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H276" s="3" t="s">
         <v>187</v>
@@ -11588,7 +11632,7 @@
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="str">
         <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
-        <v>KGC CR3H CR5-A</v>
+        <v>KGC CR3H CR4</v>
       </c>
       <c r="B277" s="3" t="s">
         <v>74</v>
@@ -11597,21 +11641,51 @@
         <v>72</v>
       </c>
       <c r="D277" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E277" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F277" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G277" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H277" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I277" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A278" s="3" t="str">
+        <f>datastore__4[[#This Row],[parent]]&amp;" "&amp;datastore__4[[#This Row],[code]]</f>
+        <v>KGC CR3H CR5-A</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D278" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E277" s="3" t="s">
+      <c r="E278" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F277" s="3" t="s">
+      <c r="F278" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G277" s="3" t="s">
+      <c r="G278" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H277" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I277" s="4" t="b">
+      <c r="H278" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I278" s="4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>